<commit_message>
✨ Versión estable: Dashboard + A/B scheduling + mejoras en bot y contexto
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\profe\OneDrive\Escritorio\WspIA\mi-bot-wsp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5CE2E5-4C53-4BD1-8174-C0B44DDAAA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE54A6AD-AB43-4EEA-9759-8FDB6AD00CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9D5F593B-F665-4884-BCEA-D568A1579BAF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="A" sheetId="1" r:id="rId1"/>
+    <sheet name="B" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="19">
   <si>
     <t xml:space="preserve">Hora </t>
   </si>
@@ -47,33 +48,9 @@
     <t>12:00 a 14:00</t>
   </si>
   <si>
-    <t>16:00 a 18:00</t>
-  </si>
-  <si>
     <t>19:30 a 21:30</t>
   </si>
   <si>
-    <t xml:space="preserve">Lunes </t>
-  </si>
-  <si>
-    <t>Martes</t>
-  </si>
-  <si>
-    <t>Miércoles</t>
-  </si>
-  <si>
-    <t>Jueves</t>
-  </si>
-  <si>
-    <t>Viernes</t>
-  </si>
-  <si>
-    <t>Sábado</t>
-  </si>
-  <si>
-    <t>Lectura</t>
-  </si>
-  <si>
     <t>Razonamiento</t>
   </si>
   <si>
@@ -90,13 +67,40 @@
   </si>
   <si>
     <t>6:00 a 8:00</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Lunes 11 de Agosto</t>
+  </si>
+  <si>
+    <t>Lectura critica</t>
+  </si>
+  <si>
+    <t>Martes 12 de Agosto</t>
+  </si>
+  <si>
+    <t>Miercoles 13 de Agosto</t>
+  </si>
+  <si>
+    <t>Jueves 14 de Agosto</t>
+  </si>
+  <si>
+    <t>Viernes 15 de Agosto</t>
+  </si>
+  <si>
+    <t>Sabado 16 de Agosto</t>
+  </si>
+  <si>
+    <t>17:10 a 18:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +116,14 @@
     </font>
     <font>
       <sz val="72"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -162,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -170,6 +182,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8A02AF-0091-4E9B-93E6-CB2826C021F1}">
   <dimension ref="C5:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,53 +530,54 @@
     <col min="7" max="7" width="27" customWidth="1"/>
     <col min="8" max="8" width="27.44140625" customWidth="1"/>
     <col min="9" max="9" width="29.88671875" customWidth="1"/>
+    <col min="10" max="10" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J6" s="1"/>
     </row>
@@ -573,19 +587,19 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J7" s="1"/>
     </row>
@@ -595,63 +609,63 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C9" s="2"/>
       <c r="D9" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C10" s="2"/>
       <c r="D10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J10" s="1"/>
     </row>
@@ -662,4 +676,168 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC7ED83-E9BD-43F0-9F32-F13EC794233B}">
+  <dimension ref="E6:L14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" customWidth="1"/>
+    <col min="9" max="9" width="17.77734375" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="5:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="5:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="5:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E8" s="2"/>
+      <c r="F8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="5:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E9" s="2"/>
+      <c r="F9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="5:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E10" s="2"/>
+      <c r="F10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="5:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E11" s="2"/>
+      <c r="F11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="14" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="G14" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E6:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>